<commit_message>
Update program input vending item file
</commit_message>
<xml_diff>
--- a/Data/Input/Vending-Items.xlsx
+++ b/Data/Input/Vending-Items.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>7up</t>
   </si>
   <si>
-    <t>Barq's</t>
-  </si>
-  <si>
     <t>Cheerwine</t>
   </si>
   <si>
@@ -31,9 +28,6 @@
     <t>Dr. Pepper</t>
   </si>
   <si>
-    <t>Java Monster</t>
-  </si>
-  <si>
     <t>Vernors Ginger Ale</t>
   </si>
   <si>
@@ -41,6 +35,27 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Barq's Root Beer</t>
+  </si>
+  <si>
+    <t>Java Monster Mean Bean</t>
+  </si>
+  <si>
+    <t>Java Monster Irish Crème</t>
+  </si>
+  <si>
+    <t>Java Monster Café Latte</t>
+  </si>
+  <si>
+    <t>Java Monster Loca Moca</t>
+  </si>
+  <si>
+    <t>Java Monster Triple Shot French Vanilla</t>
+  </si>
+  <si>
+    <t>Java Monster Triple Shot Mocha</t>
   </si>
 </sst>
 </file>
@@ -382,23 +397,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -411,7 +426,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -419,7 +434,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -427,7 +442,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -435,7 +450,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -443,7 +458,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -451,10 +466,50 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update prices in vending source document to wife's recommendations
</commit_message>
<xml_diff>
--- a/Data/Input/Vending-Items.xlsx
+++ b/Data/Input/Vending-Items.xlsx
@@ -461,7 +461,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,7 +477,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>